<commit_message>
committing test script google search
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,23 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15240" windowHeight="4050"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11775" windowHeight="2220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>TC_ID</t>
-  </si>
-  <si>
     <t>TC_Name</t>
   </si>
   <si>
@@ -42,10 +40,13 @@
     <t>Liveops_Login</t>
   </si>
   <si>
-    <t>TC_01</t>
-  </si>
-  <si>
     <t>https://qev189.qa1.liveops.com</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>TC001_TestNG_POC</t>
   </si>
 </sst>
 </file>
@@ -400,11 +401,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -412,36 +414,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>